<commit_message>
WIP - judge validations
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -31,10 +31,10 @@
     <t>Jones, Bernard</t>
   </si>
   <si>
-    <t>Anjali Abshire</t>
+    <t>Roth, Lauren</t>
   </si>
   <si>
-    <t>BVAAABSHIRE</t>
+    <t>DSUSER</t>
   </si>
 </sst>
 </file>
@@ -109,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -139,19 +139,6 @@
     </border>
     <border>
       <left/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -236,18 +223,29 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right>
-        <color indexed="8"/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -265,7 +263,7 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -277,13 +275,22 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -294,11 +301,24 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right>
-        <color indexed="8"/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -306,111 +326,70 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
-      <right>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -419,7 +398,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -432,109 +411,100 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -709,9 +679,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -791,7 +761,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -819,10 +789,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1078,9 +1048,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1368,7 +1338,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1396,10 +1366,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1674,150 +1644,150 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" t="s" s="9">
+      <c r="A2" s="7"/>
+      <c r="B2" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="11">
+      <c r="D2" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" ht="35" customHeight="1">
-      <c r="A3" t="s" s="15">
+      <c r="A3" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="16">
+      <c r="B3" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="15">
         <v>123</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>43467</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="14"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" t="s" s="22">
+      <c r="A4" s="19"/>
+      <c r="B4" t="s" s="20">
         <v>5</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="21">
         <v>123</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="22">
         <v>43498</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="14"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" t="s" s="22">
+      <c r="A5" s="19"/>
+      <c r="B5" t="s" s="20">
         <v>5</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>123</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>43498</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="14"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" t="s" s="22">
+      <c r="A6" s="19"/>
+      <c r="B6" t="s" s="20">
         <v>5</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="21">
         <v>123</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>43526</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="14"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" t="s" s="28">
+      <c r="A7" s="24"/>
+      <c r="B7" t="s" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="26">
         <v>123</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="27">
         <v>43557</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="14"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" t="s" s="32">
+      <c r="A8" s="28"/>
+      <c r="B8" t="s" s="29">
         <v>6</v>
       </c>
-      <c r="C8" t="s" s="33">
+      <c r="C8" t="s" s="30">
         <v>7</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="31">
         <v>43204</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="14"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" t="s" s="36">
+      <c r="A9" s="32"/>
+      <c r="B9" t="s" s="33">
         <v>6</v>
       </c>
-      <c r="C9" t="s" s="37">
+      <c r="C9" t="s" s="34">
         <v>7</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="35">
         <v>43205</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="14"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Judge Spreadsheet Validation (#5880)
Connects #5773 

### Description
This PR adds validation for the judge spreadsheet.

### Testing Plan
1) Download the Judge Assignments template, fill it out with fake data
1) In the rails console, run S3Service::store_file(<file_name>, <file_path>, :filepath)
1) Create a schedule period with the following command: 'JudgeSchedulePeriod.new(user: User.first, start_date: 90.days.ago, end_date: 1.days.ago, file_name: <file_name>).save!
1) Run 'SchedulePeriod.first.validate_spreadsheet', and confirm you get the expected result
1) Repeat with various errors in the spreadsheet
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Judge Non-Availability Dates</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Judge Name</t>
   </si>
   <si>
-    <t>CSS ID</t>
+    <t>CSS Id</t>
   </si>
   <si>
     <t>Date</t>
@@ -31,10 +31,13 @@
     <t>Jones, Bernard</t>
   </si>
   <si>
-    <t>Anjali Abshire</t>
+    <t>BVAJONESB</t>
   </si>
   <si>
-    <t>BVAAABSHIRE</t>
+    <t>Roth, Lauren</t>
+  </si>
+  <si>
+    <t>DSUSER</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -378,39 +381,46 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -448,13 +458,13 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -471,7 +481,7 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -489,7 +499,7 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -507,7 +517,7 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -520,7 +530,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -528,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1654,21 +1664,21 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7143" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="10.8672" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7344" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5781" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.8672" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7344" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7344" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7344" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.8672" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7344" style="1" customWidth="1"/>
-    <col min="10" max="256" width="10.7344" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47" customHeight="1">
+    <row r="1" ht="47.1" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1681,7 +1691,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" ht="32.25" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" t="s" s="9">
         <v>1</v>
@@ -1698,15 +1708,15 @@
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" ht="35" customHeight="1">
+    <row r="3" ht="35.1" customHeight="1">
       <c r="A3" t="s" s="15">
         <v>4</v>
       </c>
       <c r="B3" t="s" s="16">
         <v>5</v>
       </c>
-      <c r="C3" s="17">
-        <v>123</v>
+      <c r="C3" t="s" s="17">
+        <v>6</v>
       </c>
       <c r="D3" s="18">
         <v>43467</v>
@@ -1722,8 +1732,8 @@
       <c r="B4" t="s" s="22">
         <v>5</v>
       </c>
-      <c r="C4" s="23">
-        <v>123</v>
+      <c r="C4" t="s" s="23">
+        <v>6</v>
       </c>
       <c r="D4" s="24">
         <v>43498</v>
@@ -1739,8 +1749,8 @@
       <c r="B5" t="s" s="22">
         <v>5</v>
       </c>
-      <c r="C5" s="23">
-        <v>123</v>
+      <c r="C5" t="s" s="23">
+        <v>6</v>
       </c>
       <c r="D5" s="24">
         <v>43498</v>
@@ -1756,8 +1766,8 @@
       <c r="B6" t="s" s="22">
         <v>5</v>
       </c>
-      <c r="C6" s="23">
-        <v>123</v>
+      <c r="C6" t="s" s="23">
+        <v>6</v>
       </c>
       <c r="D6" s="24">
         <v>43526</v>
@@ -1773,8 +1783,8 @@
       <c r="B7" t="s" s="28">
         <v>5</v>
       </c>
-      <c r="C7" s="29">
-        <v>123</v>
+      <c r="C7" t="s" s="29">
+        <v>6</v>
       </c>
       <c r="D7" s="30">
         <v>43557</v>
@@ -1788,10 +1798,10 @@
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="31"/>
       <c r="B8" t="s" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s" s="33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="34">
         <v>43204</v>
@@ -1805,10 +1815,10 @@
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="35"/>
       <c r="B9" t="s" s="36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="38">
         <v>43205</v>

</xml_diff>

<commit_message>
Allow n/a for judge non-availability
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Judge Non-Availability Dates</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>860</t>
+  </si>
+  <si>
+    <t>Lamphere, Doris</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -512,6 +518,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1804,14 +1813,20 @@
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+      <c r="B10" t="s" s="37">
+        <v>9</v>
+      </c>
+      <c r="C10" s="38">
+        <v>861</v>
+      </c>
+      <c r="D10" t="s" s="37">
+        <v>10</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Allow n/a for judge non-availability (#6530)
Connects #6529 

### Description
This PR allows the hearing coordinators to upload 'N/A' for a judge's nonavailability days.

### Testing Plan
1. Upload a spreadsheet with 'N/A' listed for a judge
1. Confirm it uploads with no errors
1. Confirm the judge has an entry in NonAvailabilities with a null date
1. Confirm algorithm runs successfully
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Judge Non-Availability Dates</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>860</t>
+  </si>
+  <si>
+    <t>Lamphere, Doris</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -512,6 +518,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1804,14 +1813,20 @@
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+      <c r="B10" t="s" s="37">
+        <v>9</v>
+      </c>
+      <c r="C10" s="38">
+        <v>861</v>
+      </c>
+      <c r="D10" t="s" s="37">
+        <v>10</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixed order of first/last name
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9BB47E-4F70-1044-A384-124B684467AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A91B19-D410-5D4C-9D75-2506A9D408D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19580" yWindow="920" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Huels, Stuart</t>
-  </si>
-  <si>
-    <t>860</t>
   </si>
   <si>
     <t>Lamphere, Doris</t>
@@ -116,12 +113,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,7 +1313,7 @@
   <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1324,35 +1322,36 @@
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1" customWidth="1"/>
     <col min="9" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -1364,20 +1363,20 @@
         <v>44404</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="5">
+        <v>860</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -1389,20 +1388,20 @@
         <v>44404</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="5">
+        <v>860</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -1414,20 +1413,20 @@
         <v>44404</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3">
         <v>861</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added rspec tests for judge assignment process
</commit_message>
<xml_diff>
--- a/spec/support/validJudgeSpreadsheet.xlsx
+++ b/spec/support/validJudgeSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A91B19-D410-5D4C-9D75-2506A9D408D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1A1BDE-95F2-2A40-8EB4-3BD769E50277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="920" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21220" yWindow="1940" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
   <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>